<commit_message>
Fixed and updated coefficients.
</commit_message>
<xml_diff>
--- a/pipe/coefficients.xlsx
+++ b/pipe/coefficients.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13960" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -1396,7 +1396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="AG1" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -4999,8 +4999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5405,8 +5405,8 @@
         <v>69</v>
       </c>
       <c r="B46">
-        <f>INDEX(Constants!$B$13:$AS$13,1,ROW(A46)-2)+INDEX(Constants!$B$14:$AS$14,1,ROW(A46)-2)*Constants!$B$4*Constants!$E$4</f>
-        <v>-97421.6</v>
+        <f>INDEX(Constants!$B$13:$AS$13,1,ROW(A46)-2)+INDEX(Constants!$B$14:$AS$14,1,ROW(A46)-2)*Constants!$B$4*Constants!$E$4-Constants!AS18*Constants!AS15^2</f>
+        <v>-97421.600000024628</v>
       </c>
     </row>
     <row r="47" spans="1:2">

</xml_diff>